<commit_message>
biweekly #12 and hours stuff
</commit_message>
<xml_diff>
--- a/Hours.xlsx
+++ b/Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="205">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -648,6 +648,12 @@
   </si>
   <si>
     <t xml:space="preserve">researcher presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">worked on portfolio, recorded powerpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">submitted biweekly, alyssa’s presentation</t>
   </si>
 </sst>
 </file>
@@ -887,10 +893,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I236"/>
+  <dimension ref="A1:I238"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A219" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E237" activeCellId="0" sqref="E237"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E239" activeCellId="0" sqref="E239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.25" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -898,7 +904,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="73.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="73.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.5"/>
   </cols>
@@ -951,15 +957,15 @@
       </c>
       <c r="G2" s="4" t="n">
         <f aca="true">CEILING(NOW()-A124, 1)</f>
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H2" s="5" t="n">
-        <f aca="false">(SUM(D218:D234))*24</f>
-        <v>16</v>
+        <f aca="false">(SUM(D218:D240))*24</f>
+        <v>20.25</v>
       </c>
       <c r="I2" s="3" t="n">
         <f aca="false">H2/(G2*24)</f>
-        <v>0.00490196078431373</v>
+        <v>0.00607014388489209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5231,6 +5237,42 @@
       </c>
       <c r="E236" s="0" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="n">
+        <v>44339</v>
+      </c>
+      <c r="B237" s="2" t="n">
+        <v>0.65625</v>
+      </c>
+      <c r="C237" s="2" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D237" s="3" t="n">
+        <f aca="false">C237-B237</f>
+        <v>0.09375</v>
+      </c>
+      <c r="E237" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="1" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B238" s="2" t="n">
+        <v>0.357638888888889</v>
+      </c>
+      <c r="C238" s="2" t="n">
+        <v>0.388888888888889</v>
+      </c>
+      <c r="D238" s="3" t="n">
+        <f aca="false">C238-B238</f>
+        <v>0.03125</v>
+      </c>
+      <c r="E238" s="0" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>